<commit_message>
chore: refactor adding SMIN_SETTING as environment variable
</commit_message>
<xml_diff>
--- a/docs/sheets.xlsx
+++ b/docs/sheets.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrafifrbbn/Documents/thesis/thesis-research-2.0/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEBA88E6-946A-F947-BF51-4547A46AB61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2964302-45AA-B14E-AB4F-B9CA932286CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17140" xr2:uid="{D51652F6-4ECD-9A49-A0FB-5F5B2C039E54}"/>
+    <workbookView xWindow="840" yWindow="1160" windowWidth="28880" windowHeight="9400" activeTab="1" xr2:uid="{D51652F6-4ECD-9A49-A0FB-5F5B2C039E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fp_fits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
   <si>
     <t>Sample</t>
   </si>
@@ -99,13 +100,271 @@
   </si>
   <si>
     <t>Final number of 6dFGS galaxies</t>
+  </si>
+  <si>
+    <t>Survey: 6dFGS</t>
+  </si>
+  <si>
+    <t>New Data</t>
+  </si>
+  <si>
+    <t>Old data</t>
+  </si>
+  <si>
+    <t>Not using offset</t>
+  </si>
+  <si>
+    <t>Using offset</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1.5506 ± 0.0175</t>
+  </si>
+  <si>
+    <t>1.4382 ± 0.0173</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>-0.8051 ± 0.0044</t>
+  </si>
+  <si>
+    <t>-0.8066 ± 0.0043</t>
+  </si>
+  <si>
+    <t>rmean</t>
+  </si>
+  <si>
+    <t>0.1112 ± 0.0022</t>
+  </si>
+  <si>
+    <t>0.1033 ± 0.0023</t>
+  </si>
+  <si>
+    <t>smean</t>
+  </si>
+  <si>
+    <t>2.2391 ± 0.0015</t>
+  </si>
+  <si>
+    <t>2.2233 ± 0.0021</t>
+  </si>
+  <si>
+    <t>imean</t>
+  </si>
+  <si>
+    <t>3.3528 ± 0.0026</t>
+  </si>
+  <si>
+    <t>3.3456 ± 0.0026</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>0.0505 ± 0.0006</t>
+  </si>
+  <si>
+    <t>0.0520 ± 0.0006</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>0.3424 ± 0.0023</t>
+  </si>
+  <si>
+    <t>0.3428 ± 0.0023</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>0.1560 ± 0.0014</t>
+  </si>
+  <si>
+    <t>0.1672 ± 0.0017</t>
+  </si>
+  <si>
+    <t>1.4731 ± 0.0180</t>
+  </si>
+  <si>
+    <t>-0.8075 ± 0.0046</t>
+  </si>
+  <si>
+    <t>0.0923 ± 0.0026</t>
+  </si>
+  <si>
+    <t>2.2466 ± 0.0020</t>
+  </si>
+  <si>
+    <t>3.3622 ± 0.0030</t>
+  </si>
+  <si>
+    <t>0.0487 ± 0.0006</t>
+  </si>
+  <si>
+    <t>0.3421 ± 0.0025</t>
+  </si>
+  <si>
+    <t>0.1651 ± 0.0018</t>
+  </si>
+  <si>
+    <t>Survey: SDSS</t>
+  </si>
+  <si>
+    <t>1.4348 ± 0.0123</t>
+  </si>
+  <si>
+    <t>-0.8708 ± 0.0054</t>
+  </si>
+  <si>
+    <t>0.0448 ± 0.0028</t>
+  </si>
+  <si>
+    <t>2.2171 ± 0.0021</t>
+  </si>
+  <si>
+    <t>3.3254 ± 0.0029</t>
+  </si>
+  <si>
+    <t>0.0480 ± 0.0005</t>
+  </si>
+  <si>
+    <t>0.2920 ± 0.0025</t>
+  </si>
+  <si>
+    <t>0.1773 ± 0.0021</t>
+  </si>
+  <si>
+    <t>1.4461 ± 0.0128</t>
+  </si>
+  <si>
+    <t>-0.8758 ± 0.0057</t>
+  </si>
+  <si>
+    <t>0.0455 ± 0.0028</t>
+  </si>
+  <si>
+    <t>2.2203 ± 0.0022</t>
+  </si>
+  <si>
+    <t>3.3286 ± 0.0031</t>
+  </si>
+  <si>
+    <t>0.0477 ± 0.0005</t>
+  </si>
+  <si>
+    <t>0.2934 ± 0.0026</t>
+  </si>
+  <si>
+    <t>0.1749 ± 0.0022</t>
+  </si>
+  <si>
+    <t>1.4575 ± 0.0138</t>
+  </si>
+  <si>
+    <t>-0.8824 ± 0.0057</t>
+  </si>
+  <si>
+    <t>0.0503 ± 0.0029</t>
+  </si>
+  <si>
+    <t>2.2251 ± 0.0022</t>
+  </si>
+  <si>
+    <t>3.3297 ± 0.0031</t>
+  </si>
+  <si>
+    <t>0.0473 ± 0.0005</t>
+  </si>
+  <si>
+    <t>0.2937 ± 0.0026</t>
+  </si>
+  <si>
+    <t>0.1708 ± 0.0022</t>
+  </si>
+  <si>
+    <t>Survey: LAMOST</t>
+  </si>
+  <si>
+    <t>1.5596 ± 0.0293</t>
+  </si>
+  <si>
+    <t>-0.8246 ± 0.0093</t>
+  </si>
+  <si>
+    <t>-0.0995 ± 0.0034</t>
+  </si>
+  <si>
+    <t>2.21864 ± 0.0031</t>
+  </si>
+  <si>
+    <t>3.4467 ± 0.0038</t>
+  </si>
+  <si>
+    <t>0.0620 ± 0.0009</t>
+  </si>
+  <si>
+    <t>0.1740 ± 0.0027</t>
+  </si>
+  <si>
+    <t>1.5948 ± 0.0313</t>
+  </si>
+  <si>
+    <t>-0.8230 ± 0.0091</t>
+  </si>
+  <si>
+    <t>-0.0997 ± 0.0036</t>
+  </si>
+  <si>
+    <t>2.1883 ± 0.0035</t>
+  </si>
+  <si>
+    <t>3.4474 ± 0.0040</t>
+  </si>
+  <si>
+    <t>0.0619 ± 0.0009</t>
+  </si>
+  <si>
+    <t>0.2988 ± 0.0032</t>
+  </si>
+  <si>
+    <t>0.1748 ± 0.0031</t>
+  </si>
+  <si>
+    <t>1.5407 ± 0.0327</t>
+  </si>
+  <si>
+    <t>-0.7975 ± 0.0093</t>
+  </si>
+  <si>
+    <t>-0.0890 ± 0.0036</t>
+  </si>
+  <si>
+    <t>2.1930 ± 0.0035</t>
+  </si>
+  <si>
+    <t>3.4509 ± 0.0041</t>
+  </si>
+  <si>
+    <t>0.0630 ± 0.0009</t>
+  </si>
+  <si>
+    <t>0.2960 ± 0.0033</t>
+  </si>
+  <si>
+    <t>0.1662 ± 0.0029</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +378,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,10 +421,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,9 +459,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +499,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +605,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B292C80-FA1D-1441-978E-8A89510A93BA}">
   <dimension ref="G11:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24:G29"/>
     </sheetView>
   </sheetViews>
@@ -740,4 +1021,457 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56CDAC5-7460-EB49-B49D-4D8FC4079029}">
+  <dimension ref="C5:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="6"/>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="6"/>
+      <c r="D33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="C18:F18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
logdist analysis and add type annotation to final codes
</commit_message>
<xml_diff>
--- a/docs/sheets.xlsx
+++ b/docs/sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrafifrbbn/Documents/thesis/thesis-research-2.0/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2964302-45AA-B14E-AB4F-B9CA932286CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3270F943-3C2A-EA4E-A96C-0DBDA55EDE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1160" windowWidth="28880" windowHeight="9400" activeTab="1" xr2:uid="{D51652F6-4ECD-9A49-A0FB-5F5B2C039E54}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="30240" windowHeight="16840" activeTab="1" xr2:uid="{D51652F6-4ECD-9A49-A0FB-5F5B2C039E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>Sample</t>
   </si>
@@ -358,13 +358,19 @@
   </si>
   <si>
     <t>0.1662 ± 0.0029</t>
+  </si>
+  <si>
+    <t>chi-squared</t>
+  </si>
+  <si>
+    <t>Fundamental Plane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,6 +389,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -421,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -429,8 +441,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,9 +450,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56CDAC5-7460-EB49-B49D-4D8FC4079029}">
-  <dimension ref="C5:F41"/>
+  <dimension ref="C4:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1037,15 +1059,25 @@
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="5" t="s">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="J5" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
         <v>22</v>
@@ -1054,8 +1086,17 @@
       <c r="F6" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" ht="17" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
         <v>24</v>
@@ -1064,126 +1105,162 @@
         <v>25</v>
       </c>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="I7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <v>2675</v>
+      </c>
+      <c r="K7" s="12">
+        <v>3632</v>
+      </c>
+      <c r="L7" s="12">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="17" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="I8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="12">
+        <v>2551</v>
+      </c>
+      <c r="K8" s="12">
+        <v>2920</v>
+      </c>
+      <c r="L8" s="12">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" ht="17" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="I9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="12">
+        <v>2621</v>
+      </c>
+      <c r="K9" s="12">
+        <v>3128</v>
+      </c>
+      <c r="L9" s="12">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C19" s="6"/>
@@ -1209,13 +1286,13 @@
       <c r="C21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1223,13 +1300,13 @@
       <c r="C22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1237,13 +1314,13 @@
       <c r="C23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1251,13 +1328,13 @@
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1265,13 +1342,13 @@
       <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1279,13 +1356,13 @@
       <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1293,13 +1370,13 @@
       <c r="C27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1307,23 +1384,23 @@
       <c r="C28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C32" s="6"/>
@@ -1349,13 +1426,13 @@
       <c r="C34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1363,13 +1440,13 @@
       <c r="C35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1377,13 +1454,13 @@
       <c r="C36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1391,13 +1468,13 @@
       <c r="C37" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1405,13 +1482,13 @@
       <c r="C38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1419,13 +1496,13 @@
       <c r="C39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1433,13 +1510,13 @@
       <c r="C40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1447,18 +1524,24 @@
       <c r="C41" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="5" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:F20"/>
@@ -1466,11 +1549,6 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:F33"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>